<commit_message>
changes to bb mapping
</commit_message>
<xml_diff>
--- a/bb_mapping.xlsx
+++ b/bb_mapping.xlsx
@@ -27,6 +27,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Michael O'Connor</author>
+  </authors>
+  <commentList>
+    <comment ref="D9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael O'Connor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+note: this is not the provider key that's within the careteam key</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Michael O'Connor</author>
@@ -85,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="248">
   <si>
     <t>table</t>
   </si>
@@ -208,9 +242,6 @@
   </si>
   <si>
     <t>a provider number like an oscar number</t>
-  </si>
-  <si>
-    <t>prvdr_num</t>
   </si>
   <si>
     <t>us-npi</t>
@@ -627,17 +658,6 @@
     <t>populate src_billable_period_start, src_billable_perriod_end</t>
   </si>
   <si>
-    <t xml:space="preserve">important especially for bb_eob.src_type IN (
-       '10'  --HHA   
-       , '20' --SNF
-       , '30' --SNF
-       ,'40' --Outpatient
-       ,'50' --Hospice
-       ,'60' --Inpatient
-       ,'61' --Inpatient
-       ,'PDE'   -- part d events </t>
-  </si>
-  <si>
     <t>no data in the field yet</t>
   </si>
   <si>
@@ -645,9 +665,6 @@
   </si>
   <si>
     <t>to_char(bb_eob.src_billable_period_end, 'm-YYYY-MM') AS activity_thru_month_cd</t>
-  </si>
-  <si>
-    <t>Eng did not populate</t>
   </si>
   <si>
     <t>bb_eob_item.src_serviced_date AS activity_from_date</t>
@@ -703,9 +720,6 @@
   </si>
   <si>
     <t>an npi at fac level</t>
-  </si>
-  <si>
-    <t>fk_patient_id</t>
   </si>
   <si>
     <t>model has src_patient_reference, but I don’t see way to join to bb_patient</t>
@@ -811,6 +825,115 @@
   </si>
   <si>
     <t>needed?, likely for 'fac_proc'</t>
+  </si>
+  <si>
+    <t>#NA' AS fk_ip_stay_id</t>
+  </si>
+  <si>
+    <t>NULL AS ip_stay_from_dt</t>
+  </si>
+  <si>
+    <t>NULL AS ip_stay_thru_dt</t>
+  </si>
+  <si>
+    <t>NULL AS ip_stay_from_month_cd</t>
+  </si>
+  <si>
+    <t>NULL AS ip_stay_thru_month_cd</t>
+  </si>
+  <si>
+    <t>bb_eob, bb_eob_item, bb_eob_care_team</t>
+  </si>
+  <si>
+    <t>system: prvdr_num</t>
+  </si>
+  <si>
+    <t>change: pks, fks begin with 'cms_mssp', change to 'cms_bb' like in bb_patient (double check on this)</t>
+  </si>
+  <si>
+    <t>in Insights, the field concatenates cur_clm_uniq_id, clm_ctrl_num, clm_rndrg_prvdr_tax_num, fk_bene_id and claim from - to dates,  The 1st 3 aren't provide in BB data, so wil use bb_eob_identifier claim_id and claim_group and maybe src_provider (within eob_care_team) with the provider NPI but not all claims have care_teams.  Not sure why Insights uses the claim start end dates here insteam of claim line dates.  fk_bene_id is TBD by Eng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys'||'|'||eobidPvt.clm_id||'|'||eobidPvt.claim_group||'|'||COALESCE(bb_eob_care_team.src_provider_npi,'#NA')||'|'||bb_eob.src_patient_reference||'|'||to_char(bb_eob_item.src_serviced_period_start,'m-YYYY-MM')||'|'||to_char(bb_eob_item.src_serviced_period_end,'m-YYYY-MM') AS fk_visit_id
+</t>
+  </si>
+  <si>
+    <t>important for all src_types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coalesce(bb_eob.src_billable_period_start, bb_eob_item.src_serviced_period_start) AS visit_from_dt
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coalesce(bb_eob.src_billable_period_end, bb_eob_item.src_serviced_period_end) AS visit_thru_dt 
+</t>
+  </si>
+  <si>
+    <t>Insights uses claim level dates for these but Eng needs to populate src Billable perioid start end, so I'm coalescing with claim line level (eob_item) dates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to_char(coalesce(bb_eob.src_billable_period_start, bb_eob_item.src_serviced_period_start) ,'m-YYYY-MM') AS visit_from_month_cd
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to_char(coalesce(bb_eob.src_billable_period_end, bb_eob_item.src_serviced_period_end) ,'m-YYYY-MM') AS visit_thru_month_cd
+</t>
+  </si>
+  <si>
+    <t>fk_patient/bene_id</t>
+  </si>
+  <si>
+    <t>no sample records were loaded for Humana or Geisenger</t>
+  </si>
+  <si>
+    <t>{{dag_run.conf.org_id}}' AS org_id</t>
+  </si>
+  <si>
+    <t>{{dag_run.conf.org_id}}' AS org_id    'HUMANA'</t>
+  </si>
+  <si>
+    <t>phys'||'|'||bb_eob.pk_eob_id AS pk_activity_id</t>
+  </si>
+  <si>
+    <t>phys' AS activity_type_cd</t>
+  </si>
+  <si>
+    <t>carrier, outpatient, ?other</t>
+  </si>
+  <si>
+    <t>dme'||'|'||bb_eob.pk_eob_id AS pk_activity_id</t>
+  </si>
+  <si>
+    <t>dme' AS activity_type_cd</t>
+  </si>
+  <si>
+    <t>Eng did not populate the src_serviced_date field</t>
+  </si>
+  <si>
+    <t>#NA' AS fk_visit_id</t>
+  </si>
+  <si>
+    <t>NULL AS visit_from_dt</t>
+  </si>
+  <si>
+    <t>NULL AS visit_thru_dt</t>
+  </si>
+  <si>
+    <t>#NA' AS visit_from_month_cd</t>
+  </si>
+  <si>
+    <t>#NA' AS visit_thru_month_cd</t>
+  </si>
+  <si>
+    <t>all non carrier types, the fac types, pde (organization and facility)</t>
+  </si>
+  <si>
+    <t>Insights concatenates src_clm_srvc_prvdr_gnrc_id_num, the fk_bene_id and a clm line from date.  Tne 1st of these doesn't seem to be in the BB data (standarrd).   Organization and Facility sections carry npi information but Eng needs to add these fields.   Care_Team has npi and I'll use that for now. Eng needs to populate/create fK_bene_id and service date portions to I'll use src_patient_ref and a dummy date forr now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">med'||'|'||bb_eob_care_team.src_provider_npi||'|'||bb_eob.src_patient_reference||'|'||
+   to_char(COALESCE(bb_eob_item.src_serviced_date,CAST('1900-01-01' AS DATE)),'YYYYMMDD')
+  fk_visit_id </t>
   </si>
 </sst>
 </file>
@@ -1155,12 +1278,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1294,7 @@
     <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="92.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1220,15 +1343,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>177</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1236,10 +1359,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1264,13 +1387,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
         <v>168</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>169</v>
       </c>
-      <c r="E6" t="s">
-        <v>170</v>
+      <c r="G6" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1324,7 +1450,7 @@
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>220</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -1347,16 +1473,16 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1370,16 +1496,16 @@
         <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1390,10 +1516,10 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>230</v>
       </c>
       <c r="F12" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1401,11 +1527,20 @@
         <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1413,10 +1548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,7 +1562,7 @@
     <col min="8" max="8" width="24.28515625" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
     <col min="11" max="11" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="20.28515625" customWidth="1"/>
     <col min="17" max="17" width="18.140625" customWidth="1"/>
@@ -1437,77 +1571,85 @@
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" t="s">
         <v>127</v>
       </c>
-      <c r="F2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>171</v>
+      </c>
+      <c r="K2" t="s">
         <v>128</v>
       </c>
-      <c r="I2" t="s">
-        <v>172</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
+        <v>171</v>
+      </c>
+      <c r="N2" t="s">
         <v>129</v>
       </c>
-      <c r="L2" t="s">
-        <v>172</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q2" t="s">
         <v>130</v>
       </c>
-      <c r="O2" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>131</v>
-      </c>
       <c r="R2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="L3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="O3" s="1"/>
+        <v>186</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="Q3" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>166</v>
+        <v>165</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -1515,87 +1657,99 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F5" s="1"/>
+      <c r="K5" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:18" ht="165" x14ac:dyDescent="0.25">
+      <c r="K6" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="165" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>181</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -1603,25 +1757,25 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="R9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1629,25 +1783,25 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="R10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1655,13 +1809,22 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -1669,13 +1832,22 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -1683,13 +1855,22 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -1697,13 +1878,22 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -1711,185 +1901,252 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="225" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="233.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="165" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="165" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1897,7 +2154,7 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1905,7 +2162,7 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1913,7 +2170,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1921,7 +2178,7 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1929,7 +2186,7 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1937,7 +2194,7 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1945,7 +2202,7 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1953,7 +2210,7 @@
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1961,7 +2218,7 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1969,7 +2226,7 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1977,7 +2234,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1985,7 +2242,7 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1993,7 +2250,7 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2001,7 +2258,7 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2009,7 +2266,7 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2017,7 +2274,7 @@
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2025,7 +2282,7 @@
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2033,7 +2290,7 @@
         <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2041,7 +2298,7 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2049,7 +2306,7 @@
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2057,7 +2314,7 @@
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2065,7 +2322,7 @@
         <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2073,7 +2330,7 @@
         <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2081,7 +2338,7 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2089,7 +2346,7 @@
         <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2097,7 +2354,7 @@
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2105,7 +2362,7 @@
         <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2113,7 +2370,7 @@
         <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2121,7 +2378,7 @@
         <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2129,7 +2386,7 @@
         <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2137,7 +2394,7 @@
         <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2145,7 +2402,7 @@
         <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2153,7 +2410,7 @@
         <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2161,7 +2418,7 @@
         <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2169,7 +2426,7 @@
         <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2177,7 +2434,7 @@
         <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2185,7 +2442,7 @@
         <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2193,7 +2450,7 @@
         <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2201,7 +2458,7 @@
         <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2209,7 +2466,7 @@
         <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2217,7 +2474,7 @@
         <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2225,7 +2482,7 @@
         <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2233,7 +2490,7 @@
         <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2241,7 +2498,7 @@
         <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2249,7 +2506,7 @@
         <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2257,7 +2514,7 @@
         <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2265,7 +2522,7 @@
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2273,7 +2530,7 @@
         <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2281,7 +2538,7 @@
         <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2306,10 +2563,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2317,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2325,7 +2582,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2333,7 +2590,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2341,7 +2598,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2349,7 +2606,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2357,7 +2614,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2365,7 +2622,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2373,7 +2630,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2381,7 +2638,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2389,7 +2646,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2397,7 +2654,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2405,7 +2662,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2413,7 +2670,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2421,7 +2678,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2429,7 +2686,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2437,7 +2694,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2445,7 +2702,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2453,7 +2710,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2461,7 +2718,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2469,7 +2726,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2477,7 +2734,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2485,7 +2742,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2493,7 +2750,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2501,7 +2758,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2509,7 +2766,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2517,7 +2774,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2525,7 +2782,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2533,7 +2790,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2541,7 +2798,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2549,7 +2806,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2557,7 +2814,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2565,7 +2822,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2573,7 +2830,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2581,7 +2838,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2589,7 +2846,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2597,7 +2854,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2605,7 +2862,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2613,7 +2870,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2621,7 +2878,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2629,7 +2886,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2637,7 +2894,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2645,7 +2902,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2653,7 +2910,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2661,7 +2918,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2669,7 +2926,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2677,7 +2934,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2685,7 +2942,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2693,7 +2950,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2701,7 +2958,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2709,7 +2966,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2717,7 +2974,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2725,7 +2982,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2733,7 +2990,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2788,10 +3045,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2799,10 +3056,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2810,7 +3067,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
more changes to bb mapping
</commit_message>
<xml_diff>
--- a/bb_mapping.xlsx
+++ b/bb_mapping.xlsx
@@ -66,6 +66,30 @@
     <author>Michael O'Connor</author>
   </authors>
   <commentList>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael O'Connor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+see mapping link: https://bluebutton.cms.gov/resources/codesystem/eob-type/</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -119,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="310">
   <si>
     <t>table</t>
   </si>
@@ -613,9 +637,6 @@
  AND bb_eob_item.src_revenue IS null </t>
   </si>
   <si>
-    <t>filtering</t>
-  </si>
-  <si>
     <t>bb_eob.src_type = 'PDE'</t>
   </si>
   <si>
@@ -1093,6 +1114,40 @@
   </si>
   <si>
     <t>dspns_prvdr'||'|'||COALESCE('0123456789','#NA') AS facility_npi_num</t>
+  </si>
+  <si>
+    <t>'#NA' AS facility_place_of_service_cd</t>
+  </si>
+  <si>
+    <t>#NA' AS fk_facility_rev_ctr_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#NA' AS facility_revenue_center_cd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#NA' AS fk_tin_rendering_id </t>
+  </si>
+  <si>
+    <t>insights uses src_clm_srvc_prvdr_gnrc_id_num with qualifier code '11'.  I don’t see such fields in the BB data/spec.  Will use '#NA'</t>
+  </si>
+  <si>
+    <t>insights uses src_clm_srvc_prvdr_gnrc_id_num, src_clm_prsbng_prvdr_gnrc_id_num and qlfyr codes.  BB data and spec doesn’t have those.  BB has these provider roles:  primary, assist, supervisor, other</t>
+  </si>
+  <si>
+    <t>bb_eob_care_team</t>
+  </si>
+  <si>
+    <t>check that we're pulling from the CareTeam section of the eobs, not just providers coded as 'primary' but also as 'assist;,'supervisor','other'.   I'm only see 2 records not 'primary'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filtering
+</t>
+  </si>
+  <si>
+    <t>med'||'|'||bb_eob.pk_eob_id AS pk_activity_id</t>
+  </si>
+  <si>
+    <t>med' AS activity_type_cd</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1225,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1178,6 +1232,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1461,11 +1518,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,7 +1540,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1498,7 +1555,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G1" t="s">
         <v>17</v>
@@ -1541,10 +1598,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1555,10 +1612,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1589,16 +1646,16 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" t="s">
         <v>165</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>166</v>
       </c>
-      <c r="G6" t="s">
-        <v>167</v>
-      </c>
       <c r="I6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1626,7 +1683,7 @@
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -1661,10 +1718,10 @@
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>218</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>247</v>
+        <v>217</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="G9" t="s">
         <v>39</v>
@@ -1693,13 +1750,13 @@
         <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -1718,17 +1775,17 @@
       <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>253</v>
+      <c r="F11" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="G11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H11" t="s">
         <v>38</v>
       </c>
       <c r="I11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1742,16 +1799,16 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E12" t="s">
+        <v>254</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" t="s">
         <v>256</v>
-      </c>
-      <c r="G12" t="s">
-        <v>257</v>
       </c>
       <c r="I12" t="s">
         <v>34</v>
@@ -1768,16 +1825,16 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
+        <v>260</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G13" t="s">
         <v>261</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="G13" t="s">
-        <v>262</v>
       </c>
       <c r="I13" t="s">
         <v>34</v>
@@ -1794,10 +1851,10 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1808,7 +1865,7 @@
         <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1816,10 +1873,21 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>305</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -1838,9 +1906,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R81"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P24" sqref="P24"/>
+    <sheetView topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,31 +1932,31 @@
         <v>124</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H2" t="s">
         <v>125</v>
       </c>
       <c r="I2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K2" t="s">
         <v>126</v>
       </c>
       <c r="L2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N2" t="s">
         <v>127</v>
       </c>
       <c r="O2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q2" t="s">
         <v>128</v>
       </c>
       <c r="R2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -1898,8 +1966,8 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>161</v>
+      <c r="D3" s="5" t="s">
+        <v>307</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>159</v>
@@ -1909,20 +1977,20 @@
         <v>160</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -1933,13 +2001,16 @@
         <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="N4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>230</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -1950,14 +2021,17 @@
         <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="K5" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>235</v>
+      <c r="K5" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -1967,15 +2041,18 @@
       <c r="B6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="K6" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>236</v>
+      <c r="E6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="150" x14ac:dyDescent="0.25">
@@ -1986,28 +2063,28 @@
         <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="150" x14ac:dyDescent="0.25">
@@ -2018,28 +2095,28 @@
         <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -2050,22 +2127,22 @@
         <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2076,22 +2153,22 @@
         <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2102,19 +2179,19 @@
         <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>212</v>
+        <v>200</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2125,19 +2202,19 @@
         <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>197</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2148,19 +2225,19 @@
         <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -2171,19 +2248,19 @@
         <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -2194,19 +2271,19 @@
         <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="233.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2217,25 +2294,25 @@
         <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>221</v>
+        <v>200</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>245</v>
+        <v>219</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="135" x14ac:dyDescent="0.25">
@@ -2246,22 +2323,22 @@
         <v>59</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="135" x14ac:dyDescent="0.25">
@@ -2272,22 +2349,22 @@
         <v>60</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K18" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="N18" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2298,19 +2375,19 @@
         <v>61</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>241</v>
+        <v>225</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2321,19 +2398,19 @@
         <v>62</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="90" x14ac:dyDescent="0.25">
@@ -2344,29 +2421,29 @@
         <v>63</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="O21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="Q21" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="R21" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2376,29 +2453,29 @@
       <c r="B22" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>252</v>
+      <c r="E22" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K22" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="L22" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q22" s="3" t="s">
-        <v>292</v>
+      <c r="Q22" s="2" t="s">
+        <v>291</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -2408,29 +2485,29 @@
       <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>277</v>
+      <c r="K23" s="2" t="s">
+        <v>276</v>
       </c>
       <c r="L23" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="N23" s="3" t="s">
-        <v>277</v>
-      </c>
       <c r="O23" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>293</v>
+        <v>275</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="R23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -2440,29 +2517,29 @@
       <c r="B24" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>254</v>
+      <c r="E24" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>278</v>
+        <v>248</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q24" s="3" t="s">
-        <v>299</v>
+        <v>275</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -2472,23 +2549,29 @@
       <c r="B25" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>279</v>
+      <c r="K25" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="120" x14ac:dyDescent="0.25">
@@ -2498,23 +2581,29 @@
       <c r="B26" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>264</v>
+      <c r="E26" s="2" t="s">
+        <v>263</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>280</v>
+        <v>262</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>279</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>294</v>
+        <v>275</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="120" x14ac:dyDescent="0.25">
@@ -2524,23 +2613,29 @@
       <c r="B27" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>270</v>
+      <c r="E27" s="2" t="s">
+        <v>269</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="L27" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>296</v>
+        <v>268</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>295</v>
+        <v>275</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="60" x14ac:dyDescent="0.25">
@@ -2551,13 +2646,25 @@
         <v>70</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>284</v>
+        <v>270</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>283</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2567,17 +2674,29 @@
       <c r="B29" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>268</v>
+      <c r="E29" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -2587,17 +2706,29 @@
       <c r="B30" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>272</v>
+      <c r="E30" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>286</v>
+        <v>266</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -2608,24 +2739,39 @@
         <v>73</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
       <c r="B32" t="s">
         <v>74</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3546,7 +3692,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
more changes to bb_mapping
</commit_message>
<xml_diff>
--- a/bb_mapping.xlsx
+++ b/bb_mapping.xlsx
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="375">
   <si>
     <t>table</t>
   </si>
@@ -620,10 +620,6 @@
   </si>
   <si>
     <t>DISCHARGE_STATUS_CD_LIST</t>
-  </si>
-  <si>
-    <t>bb_eob.src_type IN ('10', '20', '30','40','50','60','61') 
- AND bb_eob_item.src_revenue IS NOT null</t>
   </si>
   <si>
     <t xml:space="preserve"> AND bb_eob.src_type IN ('10'  --HHA
@@ -1166,9 +1162,6 @@
     <t>insights uses src_clm_prvdr_spclty_cd.  Will providerSpclty at index 0</t>
   </si>
   <si>
-    <t xml:space="preserve">trim(primaryOnlyPrvdrNPILabel.providerSpclty[0]) AS provider_rendering_speecialty_cd </t>
-  </si>
-  <si>
     <t>insights uses src_rndrg_prvdr_type_cd.  Will used providerRole at index 0.  This doesn't seem correct  BB provides this: carr_line_prvdr_type_cd in an eob_careteam extension section but we're not pulling that</t>
   </si>
   <si>
@@ -1264,14 +1257,121 @@
     <t>insights uses src_clm_prsbng_prvdr_gnrc_id_num.   I don't see this in BB .. Using #NA</t>
   </si>
   <si>
-    <t>insights uses src_prvdr_prsbng_id_qlfyr_cd.  I don't see this iin BB, using '#NA;</t>
+    <t>insights uses src_prvdr_prsbng_id_qlfyr_cd.  I don't see this in BB, using '#NA;</t>
+  </si>
+  <si>
+    <t>insights uses src_ordrg_prvdr_npi_num, src_payto_prvdr_npi_num,  I do not see that the BB standard supplies these.   Will use all provider roles in careteam for now</t>
+  </si>
+  <si>
+    <t>insights uses src_ordrg_prvdr_npi_num.  I don’t; see that in the BB DME standard.  Will use providers in 'primary' roles and select the one at index 0</t>
+  </si>
+  <si>
+    <t>coalesce(trim(primaryOnlyPrvdrNPILabel.providerID[0]), 'npiNum|#NA') AS fk_provider_primary_id</t>
+  </si>
+  <si>
+    <t>'#NA' AS fk_provider_attending_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trim(primaryOnlyPrvdrNPILabel.providerSpclty[0]) AS provider_rendering_specialty_cd </t>
+  </si>
+  <si>
+    <t>insights uses src_payto_prvdr_npi_num.  I don’t seet this in BB Standard, Will again pull primary providers, selecting one at index 0</t>
+  </si>
+  <si>
+    <t>coalesce(trim(primaryOnlyPrvdrNPILabel.providerID[0]), 'npiNum|#NA') AS fk_provider_pay_to_id</t>
+  </si>
+  <si>
+    <t>coalesce(trim(primaryOnlyPrvdrNPILabel.providerID[0]), 'npiNum|#NA') AS fk_provider_ordering_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#NA' AS provider_prescribing_id_type_cd </t>
+  </si>
+  <si>
+    <t>TO_ARRAY('#NA') AS fk_diagnosis_id_list</t>
+  </si>
+  <si>
+    <t>TO_ARRAY('#NA') AS diagnosis_provider_detail_icd_9_cd_list</t>
+  </si>
+  <si>
+    <t>TO_ARRAY('#NA') AS diagnosis_provider_detail_icd_10_cd_list</t>
+  </si>
+  <si>
+    <t>hcpcs_cd'||'|'||COALESCE(bb_eob_item.src_service,'#NA') AS fk_procedure_id</t>
+  </si>
+  <si>
+    <t>insights uses COALESCE(xref.target_1_value, '#NA').   For insitution claims I don’t see where BB provides Betos, so an xref table would be ncessary here too.</t>
+  </si>
+  <si>
+    <t>COALESCE(xref.target_1_value, '#NA') AS procedure_betos_cd</t>
+  </si>
+  <si>
+    <t>insights uses 'hcpcs_cd'||'|'||COALESCE(c.src_clm_line_hcpcs_cd
+BB provides hcpcs for some EOB types  in that we capture in bb_eob_item.src_service</t>
+  </si>
+  <si>
+    <t>COALESCE(bb_eob_item.src_service,'#NA') AS procedure_hcpcs_cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bb_eob.src_type IN ('10', '20', '30','40','50','60','61') 
+</t>
+  </si>
+  <si>
+    <r>
+      <t>insights uses src_clm_line_dgns_cd, src_clm_dgns_1_cd, src_clm_dgns_##_cd
+and also src_dgns_prcdr_icd_ind to determing icd9 vs icd10
+we are pulling BB dxs inito bb_eob_diagnosis.  Eng needs to add a field capturing 'system'  which indicates icd9 vs icd10
+will pre-pend the dx's with 'icd_10_cm'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fcr now</t>
+    </r>
+  </si>
+  <si>
+    <t>insights use the above dx code field the indicator to determine icd9 vs 10.  Eng needs to pull system.  Using NA for now</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insights use the above dx code field the indicator to determine icd9 vs 10.  Eng needs to pull system. Will put all Dxs in this field for now. </t>
+  </si>
+  <si>
+    <t>allEOBDxCodeAgg.fkDiagCode AS fk_diagnosis_id_list</t>
+  </si>
+  <si>
+    <t>allEOBDxCodeAgg.diagCode AS diagnosis_provider_detail_icd_10_cd_list</t>
+  </si>
+  <si>
+    <t>insights uses COALESCE('hcpcs_cd'||'|'||c.src_clm_line_hcpcs_cd,'#NA'
+BB provides hcpcs for some EOB types  in that we capture in bb_eob_item.src_service</t>
+  </si>
+  <si>
+    <t>OALESCE('hcpcs_cd'||'|'||bb_eob_item.src_service,'#NA') AS fk_procedure_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inisghts uses COALESCE(xref.target_1_value, '#NA')
+BB for Carrier claims info around BETOS in an eob_itme_extension but Eng will have to add that and we'd need to utilize diagnosisLinkId
+for now, code using xref
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COALESCE(bb_eob_item.src_service,'#NA') AS procedure_hcpcs_cd</t>
+  </si>
+  <si>
+    <t>insights uses COALESCE(c.src_clm_line_hcpcs_cd,'#NA')
+BB provides hcpcs for some EOB types  that we capture in bb_eob_item.src_service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1317,6 +1417,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1650,8 +1758,8 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1777,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1684,7 +1792,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G1" t="s">
         <v>17</v>
@@ -1727,10 +1835,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1741,10 +1849,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1775,16 +1883,16 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
         <v>164</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>165</v>
       </c>
-      <c r="G6" t="s">
-        <v>166</v>
-      </c>
       <c r="I6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1847,10 +1955,10 @@
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G9" t="s">
         <v>39</v>
@@ -1879,13 +1987,13 @@
         <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -1905,16 +2013,16 @@
         <v>40</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H11" t="s">
         <v>38</v>
       </c>
       <c r="I11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1928,16 +2036,16 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E12" t="s">
+        <v>251</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" t="s">
         <v>253</v>
-      </c>
-      <c r="G12" t="s">
-        <v>254</v>
       </c>
       <c r="I12" t="s">
         <v>34</v>
@@ -1954,16 +2062,16 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
+        <v>257</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="G13" t="s">
         <v>258</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="G13" t="s">
-        <v>259</v>
       </c>
       <c r="I13" t="s">
         <v>34</v>
@@ -1980,10 +2088,10 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1994,7 +2102,7 @@
         <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2002,10 +2110,10 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2013,10 +2121,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2035,9 +2143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,31 +2169,31 @@
         <v>124</v>
       </c>
       <c r="F2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H2" t="s">
         <v>125</v>
       </c>
       <c r="I2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K2" t="s">
         <v>126</v>
       </c>
       <c r="L2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N2" t="s">
         <v>127</v>
       </c>
       <c r="O2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q2" t="s">
         <v>128</v>
       </c>
       <c r="R2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -2096,30 +2204,30 @@
         <v>45</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>159</v>
+        <v>364</v>
       </c>
       <c r="F3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L3" s="1"/>
       <c r="N3" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -2130,16 +2238,16 @@
         <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -2150,17 +2258,17 @@
         <v>47</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F5" s="1"/>
       <c r="K5" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -2171,17 +2279,17 @@
         <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="150" x14ac:dyDescent="0.25">
@@ -2192,28 +2300,28 @@
         <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="150" x14ac:dyDescent="0.25">
@@ -2224,28 +2332,28 @@
         <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -2256,22 +2364,22 @@
         <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2282,22 +2390,22 @@
         <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="204.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2308,19 +2416,19 @@
         <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2331,19 +2439,19 @@
         <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2354,19 +2462,19 @@
         <v>55</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -2377,19 +2485,19 @@
         <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="180" x14ac:dyDescent="0.25">
@@ -2400,19 +2508,19 @@
         <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="233.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2423,25 +2531,25 @@
         <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="135" x14ac:dyDescent="0.25">
@@ -2452,22 +2560,22 @@
         <v>59</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="135" x14ac:dyDescent="0.25">
@@ -2478,22 +2586,22 @@
         <v>60</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K18" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="N18" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2504,19 +2612,19 @@
         <v>61</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2527,19 +2635,19 @@
         <v>62</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="90" x14ac:dyDescent="0.25">
@@ -2550,29 +2658,29 @@
         <v>63</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L21" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="N21" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="O21" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="Q21" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="R21" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2583,28 +2691,28 @@
         <v>64</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K22" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="Q22" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -2615,28 +2723,28 @@
         <v>65</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="K23" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L23" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="N23" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="O23" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="R23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -2647,28 +2755,28 @@
         <v>66</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="105" x14ac:dyDescent="0.25">
@@ -2679,28 +2787,28 @@
         <v>67</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="K25" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="120" x14ac:dyDescent="0.25">
@@ -2711,28 +2819,28 @@
         <v>68</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="120" x14ac:dyDescent="0.25">
@@ -2743,28 +2851,28 @@
         <v>69</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="60" x14ac:dyDescent="0.25">
@@ -2775,25 +2883,25 @@
         <v>70</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="165" x14ac:dyDescent="0.25">
@@ -2804,28 +2912,28 @@
         <v>71</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -2836,28 +2944,28 @@
         <v>72</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -2868,28 +2976,28 @@
         <v>73</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="135" x14ac:dyDescent="0.25">
@@ -2900,25 +3008,31 @@
         <v>74</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L32" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>325</v>
       </c>
+      <c r="O32" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="Q32" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2926,22 +3040,28 @@
         <v>75</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>348</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="60" x14ac:dyDescent="0.25">
@@ -2952,22 +3072,28 @@
         <v>76</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="60" x14ac:dyDescent="0.25">
@@ -2978,19 +3104,25 @@
         <v>77</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="90" x14ac:dyDescent="0.25">
@@ -3001,19 +3133,25 @@
         <v>78</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -3024,19 +3162,25 @@
         <v>79</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -3047,19 +3191,25 @@
         <v>80</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>316</v>
+        <v>351</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="195" x14ac:dyDescent="0.25">
@@ -3070,22 +3220,28 @@
         <v>81</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -3093,22 +3249,28 @@
         <v>82</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -3116,19 +3278,25 @@
         <v>83</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>348</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -3139,22 +3307,28 @@
         <v>84</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -3165,22 +3339,28 @@
         <v>85</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="60" x14ac:dyDescent="0.25">
@@ -3191,22 +3371,28 @@
         <v>86</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -3217,74 +3403,151 @@
         <v>87</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>272</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="330" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
       <c r="B46" t="s">
         <v>88</v>
       </c>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
       <c r="B47" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
       <c r="B48" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
       <c r="B49" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E49" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="L49" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="255" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
       <c r="B50" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E50" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="L50" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
       <c r="B51" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E51" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
@@ -3292,7 +3555,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -3300,7 +3563,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -3308,7 +3571,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
@@ -3316,7 +3579,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -3324,7 +3587,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -3332,7 +3595,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -3340,7 +3603,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
@@ -3348,7 +3611,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
@@ -3356,7 +3619,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
@@ -3364,7 +3627,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
@@ -3372,7 +3635,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
@@ -3380,7 +3643,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
@@ -4050,7 +4313,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
more changes to bb mapping.xlsx
</commit_message>
<xml_diff>
--- a/bb_mapping.xlsx
+++ b/bb_mapping.xlsx
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="522">
   <si>
     <t>table</t>
   </si>
@@ -1736,82 +1736,239 @@
     <t>bb_eob_item.pk_eob_item_id AS claim_pk</t>
   </si>
   <si>
+    <t>bb_eob.src_type AS claim_type_cd</t>
+  </si>
+  <si>
+    <t>pk at item level</t>
+  </si>
+  <si>
+    <t>CASE
+          WHEN SUBSTR(bb_eob_item.src_service, 1, 1) = 'E'
+              THEN 'hcpcs_cd'||'|'||bb_eob_item.src_service
+          ELSE
+              '#NA'
+      END AS fk_dme_id</t>
+  </si>
+  <si>
+    <t>using src_service</t>
+  </si>
+  <si>
+    <t>mapped like insights using src_service but I think prependinng with 'hcpcs_cd' is wrong</t>
+  </si>
+  <si>
+    <t>CASE
+          WHEN SUBSTR(bb_eob_item.src_service, 1, 1) = 'E'
+              THEN 'hcpcs_cd'||'|'||bb_eob_item.src_service
+          ELSE
+              '#NA'
+      END AS dme_hcpcs_cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bb_eob_item.pk_eob_item_id AS claim_pk </t>
+  </si>
+  <si>
+    <t>from the cclf definition: 
+COALESCE(TO_VARCHAR(prvdr_oscar_num),'') || '|' ||
+      COALESCE(TO_VARCHAR(clm_from_dt),'') || '|' ||
+      COALESCE(TO_VARCHAR(clm_thru_dt),'') || '|' ||
+      COALESCE(TO_VARCHAR(bene_mbi_id),'')
+      AS ODS_PT_A_CLM_NK</t>
+  </si>
+  <si>
+    <t>bb_eob_procedure.pk_eob_procedure_id AS claim_pk</t>
+  </si>
+  <si>
+    <t>mapped like insights but I thing pre-pendinig with 'hcpcs_cd' is wrong</t>
+  </si>
+  <si>
+    <t>phys'||'|'||bb_eob_item.pk_eob_item_id AS pk_activity_id</t>
+  </si>
+  <si>
+    <t>dme'||'|'||bb_eob_item.pk_eob_item_id AS pk_activity_id</t>
+  </si>
+  <si>
+    <t>hcpcs_cd'||'|'||bb_eob_item.src_service AS fk_dme_id</t>
+  </si>
+  <si>
+    <t>bb_eob_item.src_service AS dme_hcpcs_cd</t>
+  </si>
+  <si>
+    <t>from the cclf definitionns: 
+COALESCE(TO_VARCHAR(clm_cntl_num),'') || '|' ||
+      COALESCE(TO_VARCHAR(bene_mbi_id),'')
+      AS ODS_PT_B_CLM_NK</t>
+  </si>
+  <si>
+    <t>from the cclf definition: 
+COALESCE(TO_VARCHAR(prvdr_oscar_num),'') || '|' ||
+      COALESCE(TO_VARCHAR(clm_from_dt),'') || '|' ||
+      COALESCE(TO_VARCHAR(clm_thru_dt),'') || '|' ||
+      COALESCE(TO_VARCHAR(bene_mbi_id),'')
+      AS ODS_PT_A_CLM_NK
+regarding prvdr_oscar_num Eng needs to pull into new field, regarding clm_from and thru Eng needs to populate src_billabl_start; and end, regarding bene_mbi Eng needs a better patient ID or fk.  in sample SQL, I'm using reference fields for now</t>
+  </si>
+  <si>
+    <t>COALESCE(TO_VARCHAR(bb_eob.src_provider_reference),'') || '|' ||
+      COALESCE(TO_VARCHAR(bb_eob.src_billable_period_start),'') || '|' ||
+      COALESCE(TO_VARCHAR(bb_eob.src_billable_period_end),'') || '|' ||
+      COALESCE(TO_VARCHAR(bb_eob.src_patient_reference),'')
+      AS ODS_PT_A_CLM_NK</t>
+  </si>
+  <si>
+    <t>from the cclf definitions 
+COALESCE(TO_VARCHAR(clm_cntl_num),'') || '|' ||
+      COALESCE(TO_VARCHAR(bene_mbi_id),'')
+      AS ODS_PT_B_CLM_NK
+for clm_cntl_num, I'm using clm_id from eob identifier section.  This aligns with BB-&gt;cclf mapping suggestion</t>
+  </si>
+  <si>
+    <t>COALESCE(TO_VARCHAR(eobidPvt.clm_id),'') || '|' ||
+      COALESCE(TO_VARCHAR(bb_eob.src_patient_reference),'')
+      AS ODS_PT_B_CLM_NK</t>
+  </si>
+  <si>
     <t>from the cclf definitioin:  COALESCE(TO_VARCHAR(clm_line_from_dt),'') || '|' ||
       COALESCE(TO_VARCHAR(prvdr_srvc_id_qlfyr_cd),'') || '|' ||
       COALESCE(TO_VARCHAR(clm_srvc_prvdr_gnrc_id_num),'') || '|' ||
       COALESCE(TO_VARCHAR(clm_dspnsng_stus_cd),'') || '|' ||
       COALESCE(TO_VARCHAR(clm_line_rx_srvc_rfrnc_num),'') || '|' ||
       COALESCE(TO_VARCHAR(clm_line_rx_fill_num),'')
+      AS ODS_PT_D_CLM_NK
+for prvdr_srvc_id_qlfyr_cd, need to access facility.identifier.system to calculate as :
+if facility.identifier.system =='http://hl7.org/fhir/sid/us-npi' then '01' else '#NA' end
+for clm_line_rx_fill_num, Eng need to create and populate a field and use bb-&gt;cclf mapping for JSON location</t>
+  </si>
+  <si>
+    <t>COALESCE(TO_VARCHAR(bb_eob_item.src_serviced_date),'') || '|' ||
+      COALESCE(TO_VARCHAR('01'),'') || '|' ||    --dummied as '01' until pull from facility.system 
+      COALESCE(TO_VARCHAR(bb_eob.src_facility_reference),'') || '|' ||  --facility field is improved in sandbox
+      COALESCE(TO_VARCHAR(bb_eob_info.src_code),'') || '|' ||
+      COALESCE(TO_VARCHAR(eobidPvt.rx_srvc_rfrnc_num),'') || '|' ||
+      COALESCE(TO_VARCHAR('02'),'')   --dummied as '2' until Eng pulls fill_num from JSON
       AS ODS_PT_D_CLM_NK</t>
   </si>
   <si>
-    <t>bb_eob.src_type AS claim_type_cd</t>
-  </si>
-  <si>
-    <t>pk at item level</t>
-  </si>
-  <si>
-    <t>CASE
-          WHEN SUBSTR(bb_eob_item.src_service, 1, 1) = 'E'
-              THEN 'hcpcs_cd'||'|'||bb_eob_item.src_service
+    <t>0.0 AS claim_line_allowed_amt</t>
+  </si>
+  <si>
+    <t>CASE 
+   WHEN SRC_CATEGORY LIKE '%clm_freq_cd' AND SRC_CODE = '8' --8:Void/cancel prior claim
+      THEN '1'
+   ELSE '0'
+    END AS src_clm_adjsmt_type_cd</t>
+  </si>
+  <si>
+    <t>this field is used internally in calculation of clm_line_paid_amt
+I used logic in a cte from bb-&gt; cclf mapping: 
+If information.[system=='https://bluebutton.cms.gov/resources/variables/clm_freq_cd'].code.coding.code == 8, then 1, else 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(CASE
+          WHEN bb_eob_info.src_clm_adjsmt_type_cd = '1'
+              THEN -1
           ELSE
-              '#NA'
-      END AS fk_dme_id</t>
-  </si>
-  <si>
-    <t>using src_service</t>
-  </si>
-  <si>
-    <t>mapped like insights using src_service but I think prependinng with 'hcpcs_cd' is wrong</t>
-  </si>
-  <si>
-    <t>CASE
-          WHEN SUBSTR(bb_eob_item.src_service, 1, 1) = 'E'
-              THEN 'hcpcs_cd'||'|'||bb_eob_item.src_service
+              1
+      END * bb_eob_item_adj.src_amount) AS claim_line_paid_amt </t>
+  </si>
+  <si>
+    <t>using cte's and similar logic as insights</t>
+  </si>
+  <si>
+    <t>0.0 AS claim_line_bene_paid_amt</t>
+  </si>
+  <si>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t>0.0 AS claim_line_paid_amt</t>
+  </si>
+  <si>
+    <t>, 0.0 AS claim_line_bene_paid_am</t>
+  </si>
+  <si>
+    <t>CASE 
+    WHEN SRC_CATEGORY LIKE '%clm_freq_cd' AND SRC_CODE = '8' --8:Void/cancel prior claim
+       THEN '1'
+    ELSE '0'
+   END AS src_clm_adjsmt_type_cd</t>
+  </si>
+  <si>
+    <t>logic used in a cte patterned after insights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(CASE
+          WHEN bb_eob_info.src_clm_adjsmt_type_cd = '1'
+              THEN -1
           ELSE
-              '#NA'
-      END AS dme_hcpcs_cd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bb_eob_item.pk_eob_item_id AS claim_pk </t>
-  </si>
-  <si>
-    <t>from the cclf definition: 
-COALESCE(TO_VARCHAR(prvdr_oscar_num),'') || '|' ||
-      COALESCE(TO_VARCHAR(clm_from_dt),'') || '|' ||
-      COALESCE(TO_VARCHAR(clm_thru_dt),'') || '|' ||
-      COALESCE(TO_VARCHAR(bene_mbi_id),'')
-      AS ODS_PT_A_CLM_NK</t>
-  </si>
-  <si>
-    <t>bb_eob_procedure.pk_eob_procedure_id AS claim_pk</t>
-  </si>
-  <si>
-    <t>mapped like insights but I thing pre-pendinig with 'hcpcs_cd' is wrong</t>
-  </si>
-  <si>
-    <t>phys'||'|'||bb_eob_item.pk_eob_item_id AS pk_activity_id</t>
-  </si>
-  <si>
-    <t>from the cclf definitions 
-COALESCE(TO_VARCHAR(clm_cntl_num),'') || '|' ||
-      COALESCE(TO_VARCHAR(bene_mbi_id),'')
-      AS ODS_PT_B_CLM_NK</t>
-  </si>
-  <si>
-    <t>dme'||'|'||bb_eob_item.pk_eob_item_id AS pk_activity_id</t>
-  </si>
-  <si>
-    <t>hcpcs_cd'||'|'||bb_eob_item.src_service AS fk_dme_id</t>
-  </si>
-  <si>
-    <t>bb_eob_item.src_service AS dme_hcpcs_cd</t>
-  </si>
-  <si>
-    <t>from the cclf definitionns: 
-COALESCE(TO_VARCHAR(clm_cntl_num),'') || '|' ||
-      COALESCE(TO_VARCHAR(bene_mbi_id),'')
-      AS ODS_PT_B_CLM_NK</t>
+              1
+      END * bb_eob_item_adj.src_amount) AS claim_line_allowed_amt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(CASE
+          WHEN bb_eob_info.src_clm_adjsmt_type_cd = '1'
+              THEN -1
+          ELSE
+              1
+      END * bb_eob_item_adj2.src_amount) AS claim_line_paid_amt </t>
+  </si>
+  <si>
+    <t>, 0.0 AS claim_line_bene_paid_amt</t>
+  </si>
+  <si>
+    <t>, 0.0 AS claim_line_allowed_amt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASE
+          WHEN bb_eob_info.src_clm_adjsmt_type_cd = '1'
+              THEN -1
+          ELSE
+              1
+      END * bb_eob_item_adj.src_amount) AS claim_line_paid_amt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(CASE
+          WHEN bb_eob_info.src_clm_adjsmt_type_cd = '1'
+              THEN -1
+          ELSE
+              1
+      END * bb_eob_item_adj.src_amount) AS claim_line_bene_paid_amt </t>
+  </si>
+  <si>
+    <t>{{dag_run.conf.load_period}}' AS load_period</t>
+  </si>
+  <si>
+    <t>according to bb-&gt;cclf mapping, this info isn’t in BB</t>
+  </si>
+  <si>
+    <t>{{ti.job_id}} AS load_run_id</t>
+  </si>
+  <si>
+    <t>, CURRENT_TIMESTAMP AS load_ts</t>
+  </si>
+  <si>
+    <t>not used in airflow script</t>
+  </si>
+  <si>
+    <t>#NA' AS claim_primary_payer_cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">according to bb-&gt;cclf mapping, this info isn’t in BB
+if we want APCs, can we lik to ref table? </t>
+  </si>
+  <si>
+    <t>#NA' AS rev_apc_hipps_cd</t>
+  </si>
+  <si>
+    <t>CURRENT_TIMESTAMP AS load_ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#NA' AS rev_apc_hipps_cd </t>
+  </si>
+  <si>
+    <t>null AS claim_primary_payer_cd</t>
+  </si>
+  <si>
+    <t>#NA' as rev_apc_hipps_cd</t>
   </si>
 </sst>
 </file>
@@ -2231,8 +2388,8 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,9 +2819,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N70" sqref="N70"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R81" sqref="R81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2783,16 +2940,16 @@
         <v>161</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>384</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>485</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>469</v>
@@ -4943,10 +5100,10 @@
         <v>109</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="F67" s="7" t="s">
         <v>475</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>476</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>467</v>
@@ -4955,10 +5112,10 @@
         <v>269</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="Q67" s="2" t="s">
         <v>467</v>
@@ -4975,10 +5132,10 @@
         <v>110</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>468</v>
@@ -4987,13 +5144,13 @@
         <v>269</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="Q68" s="2" t="s">
         <v>468</v>
@@ -5010,10 +5167,10 @@
         <v>111</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>471</v>
@@ -5028,27 +5185,42 @@
         <v>470</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="315" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>67</v>
       </c>
       <c r="B70" t="s">
         <v>112</v>
       </c>
+      <c r="E70" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="F70" s="7" t="s">
-        <v>480</v>
+        <v>487</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>488</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>490</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>484</v>
+        <v>489</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>490</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
+      </c>
+      <c r="Q70" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="R70" s="1" t="s">
-        <v>472</v>
+        <v>491</v>
       </c>
     </row>
     <row r="71" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -5059,99 +5231,330 @@
         <v>113</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>69</v>
       </c>
       <c r="B72" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E72" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="N72" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="R72" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" ht="180" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>70</v>
       </c>
       <c r="B73" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E73" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="N73" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="R73" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>71</v>
       </c>
       <c r="B74" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E74" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="N74" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="R74" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" ht="195" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
       <c r="B75" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E75" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="N75" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="R75" s="1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>73</v>
       </c>
       <c r="B76" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E76" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="K76" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="N76" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q76" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>74</v>
       </c>
       <c r="B77" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E77" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="N77" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>75</v>
       </c>
       <c r="B78" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E78" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="N78" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="Q78" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>76</v>
       </c>
       <c r="B79" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E79" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="N79" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q79" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="R79" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>77</v>
       </c>
       <c r="B80" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E80" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="I80" t="s">
+        <v>269</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="N80" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q80" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>78</v>
       </c>
       <c r="B81" t="s">
         <v>123</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q81" s="1" t="s">
+        <v>514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes - additions to bb_mapping.xlsx
</commit_message>
<xml_diff>
--- a/bb_mapping.xlsx
+++ b/bb_mapping.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="5340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="5340" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="changes or adds" sheetId="1" r:id="rId1"/>
     <sheet name="activity" sheetId="2" r:id="rId2"/>
     <sheet name="inpatient stay" sheetId="5" r:id="rId3"/>
-    <sheet name="visit" sheetId="3" r:id="rId4"/>
-    <sheet name="questions" sheetId="4" r:id="rId5"/>
-    <sheet name="SNDBX_BB BB_EOB" sheetId="6" r:id="rId6"/>
+    <sheet name="facility" sheetId="7" r:id="rId4"/>
+    <sheet name="visit" sheetId="3" r:id="rId5"/>
+    <sheet name="questions" sheetId="4" r:id="rId6"/>
+    <sheet name="SNDBX_BB BB_EOB" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -227,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="707">
   <si>
     <t>table</t>
   </si>
@@ -2146,11 +2147,6 @@
     <t>SRC_FORM</t>
   </si>
   <si>
-    <t xml:space="preserve">fac'||'|'||eob.src_provider_reference||'|'||eob.src_facility_code ||'|'||eob.src_patient_reference ||'|'||TO_CHAR(eob.src_billable_period_start,'YYYYMMDD')||'|'||TO_CHAR(eob.src_billable_period_end,'YYYYMMDD') AS pk_ip_stay_id 
-Eng  to provide a fk_bene_id in the ODS layer?
-</t>
-  </si>
-  <si>
     <t>fac' AS stay_type_cd</t>
   </si>
   <si>
@@ -2159,21 +2155,6 @@
   </si>
   <si>
     <t>same as insights</t>
-  </si>
-  <si>
-    <t>eob.src_billable_period_start AS stay_from_dt</t>
-  </si>
-  <si>
-    <t>TO_CHAR(eob.src_billable_period_start, 'm-YYYY-MM') AS stay_from_month_cd</t>
-  </si>
-  <si>
-    <t>eob.src_billable_period_end AS stay_thru_dt</t>
-  </si>
-  <si>
-    <t>TO_CHAR(eob.src_billable_period_end, 'm-YYYY-MM') AS stay_thru_month_cd</t>
-  </si>
-  <si>
-    <t>DATEDIFF('day', eob.src_billable_period_start, eob.src_billable_period_end) AS stay_length_of_stay</t>
   </si>
   <si>
     <t>insghts uses: 
@@ -2200,29 +2181,6 @@
   <si>
     <t>aggregation done at the IP stay level
 the group by needs src_clm_bill_clsfctn_cd that Eng needs to put into data model</t>
-  </si>
-  <si>
-    <t>defined the same as primary for now</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || providers.SRC_PROVIDER_NPI) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_id_list
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || case when providers.SRC_ROLE ='primary' then providers.SRC_PROVIDER_NPI end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, providers.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_primary_id_list 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || case when providers.SRC_ROLE ='primary' then providers.SRC_PROVIDER_NPI end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, providers.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_operating_id_list 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || case when providers.SRC_ROLE = 'supervisor' then providers.SRC_PROVIDER_NPI end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, providers.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_attending_id_list       
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || case when providers.SRC_ROLE in ('other','assist') then providers.SRC_PROVIDER_NPI end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, providers.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_other_id_list
-</t>
   </si>
   <si>
     <t>dspns_prvdr'||'|'||COALESCE('0123456789','#NA') AS facility_npi_num
@@ -2302,13 +2260,6 @@
     <t>trim(providers.fk_provider_primary_id_list[0]) AS fk_provider_prescribing_id</t>
   </si>
   <si>
-    <t>COALESCE(TO_VARCHAR(eob.src_provider_reference),'') || '|' ||
-      COALESCE(TO_VARCHAR(eob.src_billable_period_start),'') || '|' ||
-      COALESCE(TO_VARCHAR(eob.src_billable_period_end),'') || '|' ||
-      COALESCE(TO_VARCHAR(eob.src_patient_reference),'')
-      AS ODS_PT_A_CLM_NK</t>
-  </si>
-  <si>
     <t>could be aliased at next level</t>
   </si>
   <si>
@@ -2326,10 +2277,6 @@
   </si>
   <si>
     <t>diagnosis.&lt;for each - EXCEPT drg&gt;.extension.[url == 'https://bluebutton.cms.gov/resources/variables/clm_poa_ind_sw1'].valueCoding.code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">need a dx system inidicator. I'm prepending all the codes with 'icd_10_cm_cd' for now.  When get the indicator, add an AND to the CASE WHEN
-</t>
   </si>
   <si>
     <t>providers.fk_provider_id_list</t>
@@ -2502,6 +2449,310 @@
   </si>
   <si>
     <t>insights uses src_ordrg_prvdr_npi_num.  I don’t; see that in the BB DME standard.  Will use '#NA'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'fac'||'|'||c1.src_provider_reference||'|'||COALESCE(c1.src_facility_code,'#NA')||'|'||c1.src_patient_reference ||'|'||TO_CHAR(c1.src_billable_period_start,'YYYYMMDD')||'|'||TO_CHAR(c1.src_billable_period_end,'YYYYMMDD') AS pk_ip_stay_id 
+Eng  to provide a fk_bene_id in the ODS layer?
+facility code isn't always reliable in src_type 60, so getting null PKs
+</t>
+  </si>
+  <si>
+    <t>c1.src_billable_period_start AS stay_from_dt</t>
+  </si>
+  <si>
+    <t>TO_CHAR(c1.src_billable_period_start, 'm-YYYY-MM') AS stay_from_month_cd</t>
+  </si>
+  <si>
+    <t>c1.src_billable_period_end AS stay_thru_dt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO_CHAR(c1.src_billable_period_end, 'm-YYYY-MM') AS stay_thru_month_cd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATEDIFF('day', c1.src_billable_period_start, c1.src_billable_period_end) AS stay_length_of_stay </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARRAY_DISTINCT(ARRAY_AGG(COALESCE(eobInfoPvt.clm_ip_admsn_type_cd, '#NA'))WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, eob.src_billable_period_end DESC)) AS stay_admission_type_cd_list
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARRAY_DISTINCT(ARRAY_AGG(COALESCE(eobInfoPvt.clm_src_ip_admsn_cd, '#NA'))WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, eob.src_billable_period_end DESC)) AS stay_admission_source_cd_list
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARRAY_DISTINCT(ARRAY_AGG(COALESCE(eobInfoPvt.ptnt_dschrg_stus_cd, '#NA')) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, eob.src_billable_period_end DESC)) AS stay_discharge_status_cd_list
+</t>
+  </si>
+  <si>
+    <t>eob.src_patient_reference AS fk_bene_id 
+c1.fk_bene_id AS fk_patient_id</t>
+  </si>
+  <si>
+    <t>COALESCE(src_provider_reference,'#NA') AS src_prvdr_oscar_num 
+ccn_num'||'|'||c1.src_prvdr_oscar_num AS fk_facility_id
+    , c1.src_prvdr_oscar_num AS facility_ccn_num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COALESCE(src_provider_reference,'#NA') AS src_prvdr_oscar_num 
+c1.src_prvdr_oscar_num AS facility_ccn_num    </t>
+  </si>
+  <si>
+    <t>COALESCE(eob.src_facility_code, '#NA') AS src_fac_prvdr_npi_num
+c1.src_fac_prvdr_npi_num AS facility_npi_num</t>
+  </si>
+  <si>
+    <t>COALESCE(eob.src_facility_type,'#NA') AS src_clm_bill_fac_type_cd
+c1.src_clm_bill_fac_type_cd AS facility_type_cd</t>
+  </si>
+  <si>
+    <t>Eng need to provider the field: src_clm_bill_clsfctn_cd</t>
+  </si>
+  <si>
+    <t>defined the same as primary for now,    might be to_array('#NA')</t>
+  </si>
+  <si>
+    <t>insights uses; MAX(d.src_clm_val_sqnc_num) AS diagnosis_facility_detail_cnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insights uses: ARRAY_AGG(COALESCE(d.src_clm_poa_ind,'#NA')) WITHIN GROUP(ORDER BY d.src_clm_from_dt DESC,d.src_clm_thru_dt DESC) AS diagnosis_facility_detail_present_on_admission_cd_list
+</t>
+  </si>
+  <si>
+    <t>insights uses: ARRAY_AGG(COALESCE(d.src_clm_prod_type_cd,'#NA')) WITHIN GROUP(ORDER BY d.src_clm_from_dt DESC,d.src_clm_thru_dt DESC) AS diagnosis_facility_detail_product_type_cd_list
+per bb-&gt;cclf mapping, that field is N/A
+usiing to_array('#NA') as diagnosis_facility_detail_product_type_cd_list</t>
+  </si>
+  <si>
+    <t>to_array('#NA') as diagnosis_facility_detail_product_type_cd_list</t>
+  </si>
+  <si>
+    <t>insights uses; SUM(
+              CASE
+                  WHEN c.src_clm_adjsmt_type_cd = '1'
+                      THEN -1
+                  ELSE
+                      1
+              END * c.src_clm_pmt_amt) AS src_clm_pmt_amt</t>
+  </si>
+  <si>
+    <t>SUM(
+              CASE
+                  WHEN eobInfoPvt.clm_freq_cd = '8' --Void/cancel prior claim
+                      THEN -1
+                  ELSE
+                      1
+              END * eob.src_payment_amount) AS src_clm_pmt_amt
+c1.src_clm_pmt_amt AS claim_paid_amt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field is present in source but Eng needs to bring into model  
+(diagnosis.&lt;for each - EXCEPT drg&gt;.extension.[url == 'https://bluebutton.cms.gov/resources/variables/clm_poa_ind_sw1'].valueCoding.code)
+using this for now: to_array('#NA') AS diagnosis_facility_detail_present_on_admission_cd_list
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need a dx system inidicator. I'm prepending all the codes with 'icd_10_cm_cd' for now.  When get the indicator, add an AND to the CASE WHEN
+I have this filtering on Principal only (then concatenating Other) similar to insights, but sometimes I see admitting w/out principal so it looks weird to have a 'unfiltered' list that's blank in that case
+</t>
+  </si>
+  <si>
+    <t>insights uses: 
+ARRAY_AGG(
+              CASE
+                  WHEN COALESCE(d.src_dgns_prcdr_icd_ind,'9') = '0'
+                      THEN '#NA'
+                  ELSE
+                      COALESCE(d.src_clm_dgns_cd,'#NA')
+              END) WITHIN GROUP(ORDER BY d.src_clm_from_dt DESC,d.src_clm_thru_dt DESC) AS diagnosis_facility_detail_icd_9_cd_list</t>
+  </si>
+  <si>
+    <t>insights uses: 
+ARRAY_AGG(
+              CASE
+                  WHEN COALESCE(d.src_dgns_prcdr_icd_ind,'9') = '0'
+                      THEN COALESCE(d.src_clm_dgns_cd,'#NA')
+                  ELSE
+                      '#NA'
+              END) WITHIN GROUP(ORDER BY d.src_clm_from_dt DESC,d.src_clm_thru_dt DESC) AS diagnosis_facility_detail_icd_10_cd_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">array_distinct(array_agg(eob.src_type) WITHIN GROUP (ORDER BY eob.src_billable_period_start DESC, eob.src_billable_period_end DESC)) AS claim_type_cd_list
+</t>
+  </si>
+  <si>
+    <t>COALESCE(TO_VARCHAR(eob.src_provider_reference),'') || '|' ||
+      COALESCE(TO_VARCHAR(eob.src_billable_period_start),'') || '|' ||
+      COALESCE(TO_VARCHAR(eob.src_billable_period_end),'') || '|' ||
+      COALESCE(TO_VARCHAR(eob.src_patient_reference),'')
+      AS ODS_PT_A_CLM_NK
+c1.ods_pt_a_clm_nk AS claim_nk</t>
+  </si>
+  <si>
+    <t>0.0 AS claim_allowed_amt</t>
+  </si>
+  <si>
+    <t>1234 AS load_run_id</t>
+  </si>
+  <si>
+    <t>insights uses: src_clm_nch_prmry_pyr_cd
+per bb-&gt;cclf mapping, N/A not there</t>
+  </si>
+  <si>
+    <t>dummy number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c2 cte: 
+ARRAY_DISTINCT(ARRAY_AGG(revItem.src_revenue) WITHIN GROUP (ORDER BY eob.src_billable_period_start DESC, revItem.SRC_SEQUENCE, eob.src_billable_period_end DESC)) AS facility_revenue_center_cd_list
+final query
+c2.facility_revenue_center_cd_list
+</t>
+  </si>
+  <si>
+    <t>c4:
+ARRAY_DISTINCT(ARRAY_AGG(case when trim(diagnoses.src_type[0]['coding'][0]['code']) = 'principal' AND 1=0 then COALESCE(diagnoses.src_diagnosis_code,'#NA') 
+         else '#NA' end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, diagnoses.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as diagnosis_facility_principal_icd_9_cd_list 
+, c4.diagnosis_facility_principal_icd_9_cd_list</t>
+  </si>
+  <si>
+    <t>c4:
+ARRAY_DISTINCT(ARRAY_AGG(case when trim(diagnoses.src_type[0]['coding'][0]['code']) = 'principal' AND 1=1 then COALESCE(diagnoses.src_diagnosis_code,'#NA') 
+         else '#NA' end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, diagnoses.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as diagnosis_facility_principal_icd_10_cd_list
+c4.diagnosis_facility_principal_icd_10_cd_list</t>
+  </si>
+  <si>
+    <t>ARRAY_DISTINCT(ARRAY_AGG(case when trim(diagnoses.src_type[0]['coding'][0]['code']) = 'admitting' AND 1=0 then COALESCE(diagnoses.src_diagnosis_code,'#NA') 
+         else '#NA' end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, diagnoses.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as diagnosis_facility_admitting_icd_9_cd_list 
+c4.diagnosis_facility_admitting_icd_9_cd_list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c4:
+ARRAY_DISTINCT(ARRAY_AGG(case when trim(diagnoses.src_type[0]['coding'][0]['code']) = 'admitting' AND 1=1 then COALESCE(diagnoses.src_diagnosis_code,'#NA') 
+         else '#NA' end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, diagnoses.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as diagnosis_facility_admitting_icd_10_cd_list
+c4.diagnosis_facility_admitting_icd_10_cd_list
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c4:
+ARRAY_DISTINCT(ARRAY_AGG(case when trim(diagnoses.src_type[0]['coding'][0]['code']) = 'principal' AND 1=1 then 'icd_10_cm_cd'||'|'|| COALESCE(diagnoses.src_diagnosis_code,'#NA')
+         when trim(diagnoses.src_type[0]['coding'][0]['code']) = 'principal' AND 1=0 then 'icd_9_cm_cd'||'|'|| COALESCE(diagnoses.src_diagnosis_code,'#NA')
+         else '#NA' end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, diagnoses.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_diagnosis_id_list
+c4: 
+ARRAY_DISTINCT(ARRAY_AGG(case when trim(diagnoses.src_type[0]['coding'][0]['code']) IS NULL AND diagnoses.src_package_code IS NULL AND 1=1 then 'icd_10_cm_cd'||'|'|| COALESCE(diagnoses.src_diagnosis_code,'#NA')
+         when trim(diagnoses.src_type[0]['coding'][0]['code']) IS NULL AND diagnoses.src_package_code IS NULL AND 1=0 then 'icd_9_cm_cd'||'|'|| COALESCE(diagnoses.src_diagnosis_code,'#NA')
+         else '#NA' end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, diagnoses.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_diagnosis_id_list_other
+final query: 
+CASE
+          WHEN ARRAY_FILTER(ARRAY_CAT(c4.fk_diagnosis_id_list,COALESCE(c4.fk_diagnosis_id_list_other, array_construct())), '.*#NA$') = ARRAY_CONSTRUCT()
+              THEN TO_ARRAY('#NA')
+          ELSE ARRAY_DISTINCT(ARRAY_FILTER(ARRAY_CAT(c4.fk_diagnosis_id_list,COALESCE(c4.fk_diagnosis_id_list_other, array_construct())), '.*#NA$'))
+      END AS fk_diagnosis_id_list </t>
+  </si>
+  <si>
+    <t>c4:
+max(case when trim(diagnoses.src_type[0]['coding'][0]['code']) IS NULL AND diagnoses.src_package_code IS NULL THEN diagnoses.SRC_SEQUENCE end) AS maxSqnc
+c4.maxSqnc AS diagnosis_facility_detail_cnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c4:
+ARRAY_DISTINCT(ARRAY_AGG(case when trim(diagnoses.src_type[0]['coding'][0]['code']) IS NULL AND diagnoses.src_package_code IS NULL AND 1=0 then COALESCE(diagnoses.src_diagnosis_code,'#NA')
+         else '#NA' end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, diagnoses.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as diagnosis_facility_detail_icd_9_cd_list 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c4: 
+ARRAY_DISTINCT(ARRAY_AGG(case when trim(diagnoses.src_type[0]['coding'][0]['code']) IS NULL AND diagnoses.src_package_code IS NULL AND 1=1 then COALESCE(diagnoses.src_diagnosis_code,'#NA')
+         else '#NA' end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, diagnoses.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as diagnosis_facility_detail_icd_10_cd_list
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c4: 
+ARRAY_DISTINCT(ARRAY_AGG(diagnoses.src_package_code) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, diagnoses.SRC_SEQUENCE, eob.src_billable_period_end DESC)) AS claim_drg_cd_list 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careTeam:
+ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || coalesce(providers.SRC_PROVIDER_NPI, '#NA')) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, providers.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_id_list
+final query: 
+CASE 
+  WHEN array_filter(COALESCE(careTeam.fk_provider_id_list, array_construct()), 'npi_num\\|#NA') = array_construct() THEN TO_ARRAY('npi_num|#NA')
+  ELSE array_distinct(array_filter(careTeam.fk_provider_id_list, 'npi_num\\|#NA'))
+   END AS fk_provider_id_list
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careTeam: 
+ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || case when providers.SRC_ROLE ='primary' then providers.SRC_PROVIDER_NPI end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, providers.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_primary_id_list 
+coalesce(careTeam.fk_provider_primary_id_list, array_construct()) AS fk_provider_primary_id_list
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careTeam: 
+ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || case when providers.SRC_ROLE ='primary' then providers.SRC_PROVIDER_NPI end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, providers.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_operating_id_list 
+coalesce(careTeam.fk_provider_operating_id_list, array_construct()) AS fk_provider_operating_id_list
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careTeam: 
+ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || case when providers.SRC_ROLE = 'supervisor' then providers.SRC_PROVIDER_NPI end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, providers.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_attending_id_list       
+coalesce(careTeam.fk_provider_attending_id_list, array_construct()) AS fk_provider_attending_id_list
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">careTeam: 
+ARRAY_DISTINCT(ARRAY_AGG('npi_num' || '|' || case when providers.SRC_ROLE in ('other','assist') then providers.SRC_PROVIDER_NPI end) WITHIN GROUP(ORDER BY eob.src_billable_period_start DESC, providers.SRC_SEQUENCE, eob.src_billable_period_end DESC)) as fk_provider_other_id_list
+coalesce(careTeam.fk_provider_other_id_list, array_construct()) AS fk_provider_other_id_list
+</t>
+  </si>
+  <si>
+    <t>PK_FACILITY_ID</t>
+  </si>
+  <si>
+    <t>NUM_TYPE_CD</t>
+  </si>
+  <si>
+    <t>FACILITY_NUM</t>
+  </si>
+  <si>
+    <t>OSCAR_CCN_NUM</t>
+  </si>
+  <si>
+    <t>NPI_NUM</t>
+  </si>
+  <si>
+    <t>TAX_ID_NUM</t>
+  </si>
+  <si>
+    <t>FACILITY_SUBTYPE_CD</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>ADDR_LINE_1</t>
+  </si>
+  <si>
+    <t>ADDR_LINE_2</t>
+  </si>
+  <si>
+    <t>ADDR_CITY</t>
+  </si>
+  <si>
+    <t>ADDR_COUNTY_CD</t>
+  </si>
+  <si>
+    <t>ADDR_STATE_CD</t>
+  </si>
+  <si>
+    <t>ADDR_ZIP_CD</t>
+  </si>
+  <si>
+    <t>ADDR_POINT</t>
+  </si>
+  <si>
+    <t>FACILITY_CERTIFICATION_TYPE_CD</t>
+  </si>
+  <si>
+    <t>FACILITY_CERTIFICATION_TYPE_ROLLUP_CD</t>
   </si>
 </sst>
 </file>
@@ -2609,7 +2860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2637,6 +2888,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2921,8 +3173,8 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,7 +3330,7 @@
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -3240,7 +3492,7 @@
         <v>244</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="I13" t="s">
         <v>34</v>
@@ -3323,7 +3575,7 @@
         <v>396</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -3340,29 +3592,29 @@
         <v>398</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>282</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3370,13 +3622,13 @@
         <v>31</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>643</v>
+        <v>629</v>
       </c>
       <c r="E24" t="s">
-        <v>644</v>
+        <v>630</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>645</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -3397,9 +3649,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N21" sqref="N21"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3708,13 +3960,13 @@
         <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>197</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>646</v>
+        <v>632</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>197</v>
@@ -3847,13 +4099,13 @@
         <v>58</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>197</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>647</v>
+        <v>633</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>358</v>
@@ -3894,10 +4146,10 @@
         <v>193</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>226</v>
@@ -3920,16 +4172,16 @@
         <v>193</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>648</v>
+        <v>634</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>193</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>632</v>
+        <v>618</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>227</v>
@@ -3958,7 +4210,7 @@
         <v>193</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>228</v>
@@ -3987,7 +4239,7 @@
         <v>193</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>229</v>
@@ -4043,13 +4295,13 @@
         <v>64</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>234</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>234</v>
@@ -4067,10 +4319,10 @@
         <v>257</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>594</v>
+        <v>582</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>595</v>
+        <v>583</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="45" x14ac:dyDescent="0.25">
@@ -4081,13 +4333,13 @@
         <v>65</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>236</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>236</v>
@@ -4119,13 +4371,13 @@
         <v>66</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>235</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>235</v>
@@ -4143,7 +4395,7 @@
         <v>257</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
       <c r="R24" s="1" t="s">
         <v>276</v>
@@ -4157,13 +4409,13 @@
         <v>67</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>627</v>
+        <v>613</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>627</v>
+        <v>613</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>241</v>
@@ -4233,7 +4485,7 @@
         <v>69</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>251</v>
@@ -4371,7 +4623,7 @@
         <v>253</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>596</v>
+        <v>584</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="75" x14ac:dyDescent="0.25">
@@ -4420,31 +4672,31 @@
         <v>74</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>362</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>372</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="L32" s="6" t="s">
         <v>300</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>654</v>
+        <v>640</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>597</v>
+        <v>585</v>
       </c>
       <c r="R32" s="1" t="s">
         <v>308</v>
@@ -4461,7 +4713,7 @@
         <v>479</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>479</v>
@@ -4470,7 +4722,7 @@
         <v>373</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>287</v>
@@ -4534,13 +4786,13 @@
         <v>77</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>371</v>
@@ -4569,13 +4821,13 @@
         <v>78</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>374</v>
@@ -4616,7 +4868,7 @@
         <v>257</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>639</v>
+        <v>625</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>287</v>
@@ -4727,7 +4979,7 @@
         <v>257</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>655</v>
+        <v>641</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>315</v>
@@ -4765,7 +5017,7 @@
         <v>295</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>656</v>
+        <v>642</v>
       </c>
       <c r="Q41" s="2" t="s">
         <v>295</v>
@@ -4803,10 +5055,10 @@
         <v>257</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>642</v>
+        <v>628</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="240" x14ac:dyDescent="0.25">
@@ -4841,10 +5093,10 @@
         <v>257</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="90" x14ac:dyDescent="0.25">
@@ -4879,10 +5131,10 @@
         <v>257</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>606</v>
+        <v>594</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>603</v>
+        <v>591</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="90" x14ac:dyDescent="0.25">
@@ -4917,10 +5169,10 @@
         <v>257</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>605</v>
+        <v>593</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="330" x14ac:dyDescent="0.25">
@@ -5203,10 +5455,10 @@
         <v>249</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>651</v>
+        <v>637</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>652</v>
+        <v>638</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>342</v>
@@ -5241,7 +5493,7 @@
         <v>249</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>653</v>
+        <v>639</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>347</v>
@@ -5276,7 +5528,7 @@
         <v>367</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>367</v>
@@ -5816,7 +6068,7 @@
         <v>441</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>640</v>
+        <v>626</v>
       </c>
       <c r="R70" s="1" t="s">
         <v>446</v>
@@ -6167,14 +6419,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E49"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="25.140625" customWidth="1"/>
@@ -6185,7 +6437,7 @@
         <v>504</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -6219,7 +6471,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -6230,10 +6482,10 @@
         <v>483</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>573</v>
+        <v>643</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -6247,10 +6499,10 @@
         <v>483</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -6264,7 +6516,7 @@
         <v>487</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>577</v>
+        <v>644</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -6278,7 +6530,7 @@
         <v>483</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>578</v>
+        <v>645</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -6292,7 +6544,7 @@
         <v>487</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>579</v>
+        <v>646</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -6306,7 +6558,7 @@
         <v>483</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>580</v>
+        <v>647</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -6320,10 +6572,10 @@
         <v>492</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -6333,11 +6585,14 @@
       <c r="C12" t="s">
         <v>494</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>649</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -6347,8 +6602,11 @@
       <c r="C13" t="s">
         <v>494</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>650</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6362,10 +6620,10 @@
         <v>483</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -6375,8 +6633,11 @@
       <c r="C15" t="s">
         <v>494</v>
       </c>
+      <c r="D15" s="1" t="s">
+        <v>651</v>
+      </c>
       <c r="E15" s="1" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -6390,10 +6651,10 @@
         <v>483</v>
       </c>
       <c r="D16" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -6403,8 +6664,11 @@
       <c r="C17" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -6414,8 +6678,11 @@
       <c r="C18" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -6425,8 +6692,11 @@
       <c r="C19" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -6436,8 +6706,11 @@
       <c r="C20" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -6447,8 +6720,11 @@
       <c r="C21" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -6458,8 +6734,14 @@
       <c r="C22" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -6469,8 +6751,11 @@
       <c r="C23" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -6481,13 +6766,13 @@
         <v>494</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>588</v>
+        <v>685</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="390" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -6498,13 +6783,13 @@
         <v>494</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>589</v>
+        <v>686</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -6515,13 +6800,13 @@
         <v>494</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>590</v>
+        <v>687</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -6532,10 +6817,10 @@
         <v>494</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="285" x14ac:dyDescent="0.25">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -6546,10 +6831,10 @@
         <v>494</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -6559,11 +6844,14 @@
       <c r="C29" t="s">
         <v>494</v>
       </c>
+      <c r="D29" s="1" t="s">
+        <v>680</v>
+      </c>
       <c r="E29" s="1" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -6573,8 +6861,11 @@
       <c r="C30" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="375" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -6584,8 +6875,11 @@
       <c r="C31" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -6595,8 +6889,11 @@
       <c r="C32" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -6606,8 +6903,11 @@
       <c r="C33" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -6617,8 +6917,14 @@
       <c r="C34" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="240" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -6628,8 +6934,14 @@
       <c r="C35" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -6639,9 +6951,14 @@
       <c r="C36" t="s">
         <v>494</v>
       </c>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -6651,8 +6968,14 @@
       <c r="C37" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -6661,6 +6984,12 @@
       </c>
       <c r="C38" t="s">
         <v>494</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="135" x14ac:dyDescent="0.25">
@@ -6674,10 +7003,10 @@
         <v>494</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -6688,13 +7017,13 @@
         <v>483</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>607</v>
+        <v>670</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -6704,8 +7033,11 @@
       <c r="C41" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -6715,8 +7047,11 @@
       <c r="C42" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -6726,8 +7061,14 @@
       <c r="C43" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E43" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
@@ -6737,8 +7078,14 @@
       <c r="C44" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
@@ -6748,8 +7095,11 @@
       <c r="C45" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
@@ -6759,8 +7109,14 @@
       <c r="C46" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="11" t="s">
+        <v>672</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
@@ -6770,8 +7126,11 @@
       <c r="C47" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
@@ -6781,8 +7140,14 @@
       <c r="C48" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -6791,6 +7156,9 @@
       </c>
       <c r="C49" t="s">
         <v>483</v>
+      </c>
+      <c r="D49" t="s">
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -6801,6 +7169,288 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C3" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>690</v>
+      </c>
+      <c r="C5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>691</v>
+      </c>
+      <c r="C6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>692</v>
+      </c>
+      <c r="C7" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>693</v>
+      </c>
+      <c r="C8" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>694</v>
+      </c>
+      <c r="C9" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>695</v>
+      </c>
+      <c r="C11" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>696</v>
+      </c>
+      <c r="C13" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>697</v>
+      </c>
+      <c r="C14" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>698</v>
+      </c>
+      <c r="C15" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>699</v>
+      </c>
+      <c r="C16" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>700</v>
+      </c>
+      <c r="C17" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>701</v>
+      </c>
+      <c r="C18" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>702</v>
+      </c>
+      <c r="C19" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>703</v>
+      </c>
+      <c r="C20" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>704</v>
+      </c>
+      <c r="C21" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>705</v>
+      </c>
+      <c r="C25" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>706</v>
+      </c>
+      <c r="C26" t="s">
+        <v>483</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B55"/>
   <sheetViews>
@@ -7250,7 +7900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -7330,12 +7980,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed to bb mapping
</commit_message>
<xml_diff>
--- a/bb_mapping.xlsx
+++ b/bb_mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="5340" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16920" windowHeight="5340" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="changes or adds" sheetId="1" r:id="rId1"/>
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1311" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="764">
   <si>
     <t>table</t>
   </si>
@@ -2753,6 +2753,284 @@
   </si>
   <si>
     <t>FACILITY_CERTIFICATION_TYPE_ROLLUP_CD</t>
+  </si>
+  <si>
+    <t>filtering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c1.src_type IN ('10'  --HHA
+       , '20' --SNF
+       , '30' --SNF
+       ,'40' --Outpatient
+       ,'50' --Hospice
+       ,'60' --Inpatient
+       ,'61' --Inpatient
+       ,'81' --dme
+       ,'82' --dme
+       ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tin'||'|'||'#NA' AS pk_facility_id </t>
+  </si>
+  <si>
+    <t>c7.src_type = 'PDE'</t>
+  </si>
+  <si>
+    <t>claims: 
+DISTINCT 'dspns_prvdr' AS num_type_cd
+  , CASE 
+   WHEN c7.src_facility_code_type_reference = 'http://hl7.org/fhir/sid/us-npi'
+    THEN 'npi_num'
+   --don't have any examples of the systems for UPIN/06 or NCPDP/07 or tin
+   ELSE '#NA'
+   END || '|' || COALESCE(c7.src_facility_code,'#NA') AS facility_num 
+final select: 
+claims.num_type_cd||'|'||claims.facility_num AS pk_facility_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c5.src_type IN ('71'  
+       , '72')
+this section of etl relies on clm_rndrg_prvdr_tax_num which is not provided by blue button.  Do we remove the section? </t>
+  </si>
+  <si>
+    <t>join condition: 
+FROM local_chrisfreyder.sndbx_bb.bb_EOB c1, 
+         lateral flatten(array_construct(
+               COALESCE(src_provider_reference, '#NA')
+             , COALESCE(src_facility_code, '#NA')
+         )) c1t
+CASE
+          WHEN c1t.index = 0
+              THEN 'ccn_num'
+          ELSE
+              'npi_num'
+      END || '|' || c1t.value AS pk_facility_id</t>
+  </si>
+  <si>
+    <t>CASE
+          WHEN c1t.index = 0
+              THEN 'ccn_num'
+          ELSE
+              'npi_num'
+      END AS num_type_cd</t>
+  </si>
+  <si>
+    <t>tin' AS num_type_cd</t>
+  </si>
+  <si>
+    <t>claims.num_type_cd</t>
+  </si>
+  <si>
+    <t>claims: 
+c1t.value AS facility_num</t>
+  </si>
+  <si>
+    <t>#NA' AS facility_num</t>
+  </si>
+  <si>
+    <t>claims.facility_num</t>
+  </si>
+  <si>
+    <t>CASE
+          WHEN c1t.index = 0
+              THEN c1t.value
+          ELSE
+              '#NA'
+      END AS oscar_ccn_num</t>
+  </si>
+  <si>
+    <t>#NA' AS oscar_ccn_num</t>
+  </si>
+  <si>
+    <t>CASE
+          WHEN c1t.index = 1
+              THEN c1t.value
+          ELSE
+              '#NA'
+      END AS npi_num</t>
+  </si>
+  <si>
+    <t>#NA' AS npi_num</t>
+  </si>
+  <si>
+    <t>claims: 
+CASE
+        WHEN c7.src_facility_code_type_reference = 'http://hl7.org/fhir/sid/us-npi'
+            THEN COALESCE(c7.src_facility_code,'#NA')
+        ELSE
+            '#NA'
+           END AS npi_num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">od: 
+ SELECT
+        src_facility_ccn
+        ,src_tin
+     FROM prod_humana.ods.nh_network_model_3_fac nsf3
+final query: 
+od.src_tin AS fk_tin_id
+</t>
+  </si>
+  <si>
+    <t>final query: 
+COALESCE(od.src_tin, '#NA') AS tax_id_num</t>
+  </si>
+  <si>
+    <t>insights uses: COALESCE(c5.src_clm_rndrg_prvdr_tax_num,'#NA') AS tax_id_num</t>
+  </si>
+  <si>
+    <t>insights uses: COALESCE(c5.src_clm_rndrg_prvdr_tax_num,'#NA') AS facility_num</t>
+  </si>
+  <si>
+    <t>insights uses: 'tin'||'|'||COALESCE(c5.src_clm_rndrg_prvdr_tax_num,'#NA') AS pk_facility_id</t>
+  </si>
+  <si>
+    <t>NULL AS fk_tin_id</t>
+  </si>
+  <si>
+    <t>#NA' AS tax_id_num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes: </t>
+  </si>
+  <si>
+    <t>insights uses: 
+claims: 
+CASE
+              WHEN c7.src_prvdr_srvc_id_qlfyr_cd = '11'
+                  THEN COALESCE(c7.src_clm_srvc_prvdr_gnrc_id_num,'#NA')
+              ELSE
+                  '#NA'
+          END AS tin
+final query:
+claims.tin AS tax_id_num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">claims: 
+, '#NA' AS tin
+ --don't have any examples of the systems for tin
+ --   CASE
+ --              WHEN c7.src_prvdr_srvc_id_qlfyr_cd = '11'
+ --                  THEN COALESCE(c7.src_clm_srvc_prvdr_gnrc_id_num,'#NA')
+ --              ELSE
+ --                  '#NA'
+ --          END AS tin </t>
+  </si>
+  <si>
+    <t>fo: 
+SELECT
+        , od_ccn.prvdr_ctgry_cd AS fac_type_cd
+        , od_ccn.prvdr_ctgry_cd||'-'||od_ccn.prvdr_ctgry_sbtyp_cd AS fac_subtype_cd
+    FROM {{env}}_common.od.od_ccn_prvdr_service_reg_201609 od_ccn
+final query: 
+COALESCE(fo.fac_type_cd, '#NA') AS facility_type_cd</t>
+  </si>
+  <si>
+    <t>final query: 
+COALESCE(fo.fac_subtype_cd, '#NA') AS facility_subtype_cd</t>
+  </si>
+  <si>
+    <t>#NA' AS facility_subtype_cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fo: 
+od_ccn.fac_name AS name
+fn: 
+SELECT 
+COALESCE(TRIM(od_npi.prov_org_name_legal_business_name), TRIM(COALESCE(od_npi.prov_name_prefix_text||' ','')||COALESCE(od_npi.prov_first_name,'')||COALESCE(' '||od_npi.prov_middle_name,'')||COALESCE(' '||od_npi.prov_last_name_legal_name,'')||COALESCE(' '||od_npi.prov_name_suffix_text,'')||COALESCE(', '||od_npi.prov_cred_text,'')),'unknown') AS name
+FROM {{env}}_common.od.od_npi_nppes_data od_npi
+union distinct
+SELECT
+COALESCE(od_rehab.name,'Unknown') AS name
+FROM {{env}}_common.od.od_hosp_rehab_facility_2017 od_rehab
+final query:COALESCE(fo.name, fn.name, 'unknown') AS name
+</t>
+  </si>
+  <si>
+    <t>physician tin ['||'#NA'||']' AS NAME</t>
+  </si>
+  <si>
+    <t>fn: 
+SELECT 
+COALESCE(TRIM(od_npi.prov_org_name_legal_business_name), TRIM(COALESCE(od_npi.prov_name_prefix_text||' ','')||COALESCE(od_npi.prov_first_name,'')||COALESCE(' '||od_npi.prov_middle_name,'')||COALESCE(' '||od_npi.prov_last_name_legal_name,'')||COALESCE(' '||od_npi.prov_name_suffix_text,'')||COALESCE(', '||od_npi.prov_cred_text,'')),'unknown') AS name
+FROM {{env}}_common.od.od_npi_nppes_data od_npi
+union distinct
+SELECT
+COALESCE(od_rehab.name,'Unknown') AS name
+FROM {{env}}_common.od.od_hosp_rehab_facility_2017 od_rehab
+final query: 
+COALESCE(fn.name, 'dispensing provider ['||claims.facility_num||']') AS name</t>
+  </si>
+  <si>
+    <t>COALESCE(fo.addr_line_1, fn.addr_line_1, 'unknown') AS addr_line_1</t>
+  </si>
+  <si>
+    <t>COALESCE(fn.addr_line_2, 'unknown') AS addr_line_2</t>
+  </si>
+  <si>
+    <t>COALESCE(fo.addr_city, fn.addr_city, 'unknown') AS addr_city</t>
+  </si>
+  <si>
+    <t>COALESCE(fo.addr_county_cd, '#NA') AS addr_county_cd</t>
+  </si>
+  <si>
+    <t>COALESCE(fo.addr_state_cd, fn.addr_state_cd, '#NA') AS addr_state_cd</t>
+  </si>
+  <si>
+    <t>COALESCE(fo.addr_zip_cd, fn.addr_zip_cd, '#NA') AS addr_zip_cd</t>
+  </si>
+  <si>
+    <t>NULL AS addr_point</t>
+  </si>
+  <si>
+    <t>fac_type_3_4 and fac_typ_3_1  created from {env}}_common.ref.code_xref_map
+COALESCE(fac_type_3_4.target_1_value,fac_type_3_1.target_1_value) facility_certification_type_cd</t>
+  </si>
+  <si>
+    <t>COALESCE(fac_type_3_4.target_2_value,fac_type_3_1.target_2_value) AS facility_certification_type_rollup_cd</t>
+  </si>
+  <si>
+    <t>#NA' AS facility_certification_type_cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#NA' AS facility_certification_type_rollup_cd
+    , </t>
+  </si>
+  <si>
+    <t>#NA'  AS addr_line_1</t>
+  </si>
+  <si>
+    <t>#NA'  AS addr_line_2</t>
+  </si>
+  <si>
+    <t>#NA'  AS addr_city</t>
+  </si>
+  <si>
+    <t>#NA' AS addr_county_cd</t>
+  </si>
+  <si>
+    <t>#NA' AS addr_state_cd</t>
+  </si>
+  <si>
+    <t>#NA' AS addr_zip_cd</t>
+  </si>
+  <si>
+    <t>NULL  AS addr_point</t>
+  </si>
+  <si>
+    <t>COALESCE(fn.addr_line_1, 'unknown') AS addr_line_1</t>
+  </si>
+  <si>
+    <t>unknown' AS addr_line_2</t>
+  </si>
+  <si>
+    <t>COALESCE(fn.addr_city, 'unknown') AS addr_city</t>
+  </si>
+  <si>
+    <t>COALESCE(fn.addr_state_cd, '#NA') AS addr_state_cd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> COALESCE(fn.addr_zip_cd, '#NA') AS addr_zip_cd</t>
   </si>
 </sst>
 </file>
@@ -2860,7 +3138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2889,6 +3167,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3649,9 +3933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R81"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6419,7 +6703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -7170,18 +7454,43 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C26"/>
+  <dimension ref="A2:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" customWidth="1"/>
+    <col min="11" max="11" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>707</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="H2" t="s">
+        <v>732</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>480</v>
       </c>
@@ -7192,7 +7501,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -7202,8 +7511,17 @@
       <c r="C4" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="330" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -7213,8 +7531,21 @@
       <c r="C5" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>729</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="1" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -7224,8 +7555,17 @@
       <c r="C6" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="J6" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -7235,8 +7575,21 @@
       <c r="C7" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>728</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -7246,8 +7599,17 @@
       <c r="C8" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -7257,8 +7619,17 @@
       <c r="C9" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -7268,8 +7639,17 @@
       <c r="C10" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="J10" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="225" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -7279,8 +7659,24 @@
       <c r="C11" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>727</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -7290,8 +7686,17 @@
       <c r="C12" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -7301,8 +7706,17 @@
       <c r="C13" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -7312,8 +7726,17 @@
       <c r="C14" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -7323,8 +7746,17 @@
       <c r="C15" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -7334,8 +7766,17 @@
       <c r="C16" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -7345,8 +7786,17 @@
       <c r="C17" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -7356,8 +7806,17 @@
       <c r="C18" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -7367,8 +7826,17 @@
       <c r="C19" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -7378,8 +7846,17 @@
       <c r="C20" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -7389,8 +7866,17 @@
       <c r="C21" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>747</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -7400,8 +7886,17 @@
       <c r="C22" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -7411,8 +7906,17 @@
       <c r="C23" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -7422,8 +7926,17 @@
       <c r="C24" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -7433,8 +7946,17 @@
       <c r="C25" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -7444,9 +7966,19 @@
       <c r="C26" t="s">
         <v>483</v>
       </c>
+      <c r="E26" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>751</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>